<commit_message>
Update generated bank statements and ground truth CSV
- Modified PNG and XLSX files for statements 1-132
- Updated ground_truth.csv with new reference data
- Ensures consistency in generated bank statement samples for testing or validation purposes
</commit_message>
<xml_diff>
--- a/bank statement generator/bank_statements/statement_1.xlsx
+++ b/bank statement generator/bank_statements/statement_1.xlsx
@@ -682,7 +682,7 @@
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
-          <t>Engin</t>
+          <t>Hartmut</t>
         </is>
       </c>
       <c r="D2" s="8" t="n"/>
@@ -699,12 +699,12 @@
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="8" t="inlineStr">
         <is>
-          <t>2267041356247526</t>
+          <t>2570314725427075</t>
         </is>
       </c>
       <c r="C3" s="8" t="inlineStr">
         <is>
-          <t>Peukert</t>
+          <t>Mohaupt</t>
         </is>
       </c>
       <c r="D3" s="8" t="n"/>
@@ -751,7 +751,7 @@
       <c r="C5" s="8" t="n"/>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>KONTOSTAND AM 03.06.2024</t>
+          <t>KONTOSTAND AM 08.04.2025</t>
         </is>
       </c>
       <c r="E5" s="17" t="n"/>
@@ -759,130 +759,146 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="B6" s="8" t="inlineStr">
         <is>
-          <t>07.06.</t>
+          <t>11.04.</t>
         </is>
       </c>
       <c r="C6" s="8" t="inlineStr">
         <is>
-          <t>08.06.</t>
+          <t>12.04.</t>
         </is>
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>BEITRAG Allianz SE K-71445329</t>
+          <t>KARTENZ./11.04 EDEKA RO</t>
         </is>
       </c>
       <c r="E6" s="17" t="inlineStr">
         <is>
-          <t>56,28-</t>
+          <t>64,97-</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="8" t="inlineStr">
         <is>
-          <t>08.06.</t>
+          <t>13.04.</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
         <is>
-          <t>09.06.</t>
+          <t>14.04.</t>
         </is>
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>BURGER KING Vilsbiburg</t>
+          <t>MCDONALDS Seelow</t>
         </is>
       </c>
       <c r="E7" s="17" t="inlineStr">
         <is>
-          <t>34,35-</t>
+          <t>35,81-</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="8" t="inlineStr">
         <is>
-          <t>11.06.</t>
+          <t>16.04.</t>
         </is>
       </c>
       <c r="C8" s="8" t="inlineStr">
         <is>
-          <t>12.06.</t>
+          <t>17.04.</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>RECHNUNG VODAFONE GMBH 2925470</t>
+          <t>BURGER KING Wismar</t>
         </is>
       </c>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>39,63-</t>
+          <t>16,75-</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="8" t="inlineStr">
         <is>
-          <t>12.06.</t>
+          <t>18.04.</t>
         </is>
       </c>
       <c r="C9" s="8" t="inlineStr">
         <is>
-          <t>13.06.</t>
+          <t>19.04.</t>
         </is>
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>KARTENZAHLUNG JET TANKSTELLE</t>
+          <t>MITGLIEDSBEITRAG ZEUS BODYPOWER</t>
         </is>
       </c>
       <c r="E9" s="17" t="inlineStr">
         <is>
-          <t>65,62-</t>
+          <t>25,12-</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="8" t="inlineStr">
         <is>
-          <t>15.06.</t>
+          <t>21.04.</t>
         </is>
       </c>
       <c r="C10" s="8" t="inlineStr">
         <is>
-          <t>16.06.</t>
+          <t>22.04.</t>
         </is>
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>KARTENZAHLUNG JET TANKSTELLE</t>
+          <t>PAYPAL XUBVUF</t>
         </is>
       </c>
       <c r="E10" s="17" t="inlineStr">
         <is>
-          <t>52,18-</t>
+          <t>72,41-</t>
         </is>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="8" t="n"/>
-      <c r="C11" s="8" t="n"/>
-      <c r="D11" s="8" t="n"/>
-      <c r="E11" s="12" t="n"/>
+      <c r="B11" s="8" t="inlineStr">
+        <is>
+          <t>23.04.</t>
+        </is>
+      </c>
+      <c r="C11" s="8" t="inlineStr">
+        <is>
+          <t>24.04.</t>
+        </is>
+      </c>
+      <c r="D11" s="8" t="inlineStr">
+        <is>
+          <t>BEITRAG Allianz SE K-29921652</t>
+        </is>
+      </c>
+      <c r="E11" s="17" t="inlineStr">
+        <is>
+          <t>55,76-</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="27.75" customHeight="1">
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="8" t="n"/>
       <c r="D12" s="9" t="inlineStr">
         <is>
-          <t>KONTOSTAND AM 18.06.2024</t>
+          <t>KONTOSTAND AM 28.04.2025</t>
         </is>
       </c>
       <c r="E12" s="17" t="inlineStr">
         <is>
-          <t>248,06-</t>
+          <t>270,82-</t>
         </is>
       </c>
     </row>
@@ -890,7 +906,7 @@
       <c r="B13" s="11" t="n"/>
       <c r="C13" s="11" t="inlineStr">
         <is>
-          <t>IHR NAECHSTER ABRECHNUNGSTERMIN 26.06.2024</t>
+          <t>IHR NAECHSTER ABRECHNUNGSTERMIN 04.05.2025</t>
         </is>
       </c>
       <c r="D13" s="11" t="n"/>

</xml_diff>